<commit_message>
Fix mistakes in number of regional test cases
</commit_message>
<xml_diff>
--- a/data/03_covid_tests/regional_tests.xlsx
+++ b/data/03_covid_tests/regional_tests.xlsx
@@ -409,7 +409,7 @@
         <v>1792</v>
       </c>
       <c r="D2">
-        <v>1792</v>
+        <v>57</v>
       </c>
       <c r="E2">
         <v>15071</v>
@@ -431,7 +431,7 @@
         <v>337</v>
       </c>
       <c r="D3">
-        <v>337</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>11685</v>
@@ -453,7 +453,7 @@
         <v>1557</v>
       </c>
       <c r="D4">
-        <v>1557</v>
+        <v>98</v>
       </c>
       <c r="E4">
         <v>59468</v>
@@ -475,7 +475,7 @@
         <v>330</v>
       </c>
       <c r="D5">
-        <v>330</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>21540</v>
@@ -497,7 +497,7 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>13279</v>
@@ -519,7 +519,7 @@
         <v>40</v>
       </c>
       <c r="D7">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>11348</v>
@@ -541,7 +541,7 @@
         <v>2089</v>
       </c>
       <c r="D8">
-        <v>2089</v>
+        <v>118</v>
       </c>
       <c r="E8">
         <v>57911</v>
@@ -563,7 +563,7 @@
         <v>457</v>
       </c>
       <c r="D9">
-        <v>457</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>21210</v>
@@ -585,7 +585,7 @@
         <v>119</v>
       </c>
       <c r="D10">
-        <v>119</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>13268</v>
@@ -607,7 +607,7 @@
         <v>173</v>
       </c>
       <c r="D11">
-        <v>173</v>
+        <v>4</v>
       </c>
       <c r="E11">
         <v>11308</v>
@@ -629,7 +629,7 @@
         <v>1254</v>
       </c>
       <c r="D12">
-        <v>1254</v>
+        <v>101</v>
       </c>
       <c r="E12">
         <v>55822</v>
@@ -651,7 +651,7 @@
         <v>297</v>
       </c>
       <c r="D13">
-        <v>297</v>
+        <v>8</v>
       </c>
       <c r="E13">
         <v>20753</v>
@@ -673,7 +673,7 @@
         <v>182</v>
       </c>
       <c r="D14">
-        <v>182</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>13149</v>
@@ -695,7 +695,7 @@
         <v>408</v>
       </c>
       <c r="D15">
-        <v>408</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <v>11135</v>
@@ -717,7 +717,7 @@
         <v>1479</v>
       </c>
       <c r="D16">
-        <v>1479</v>
+        <v>147</v>
       </c>
       <c r="E16">
         <v>54568</v>
@@ -739,7 +739,7 @@
         <v>686</v>
       </c>
       <c r="D17">
-        <v>686</v>
+        <v>34</v>
       </c>
       <c r="E17">
         <v>20456</v>
@@ -761,7 +761,7 @@
         <v>244</v>
       </c>
       <c r="D18">
-        <v>244</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>12967</v>
@@ -783,7 +783,7 @@
         <v>329</v>
       </c>
       <c r="D19">
-        <v>329</v>
+        <v>10</v>
       </c>
       <c r="E19">
         <v>10727</v>
@@ -805,7 +805,7 @@
         <v>2223</v>
       </c>
       <c r="D20">
-        <v>2223</v>
+        <v>157</v>
       </c>
       <c r="E20">
         <v>53089</v>
@@ -827,7 +827,7 @@
         <v>420</v>
       </c>
       <c r="D21">
-        <v>420</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <v>19770</v>
@@ -849,7 +849,7 @@
         <v>144</v>
       </c>
       <c r="D22">
-        <v>144</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <v>12723</v>
@@ -871,7 +871,7 @@
         <v>387</v>
       </c>
       <c r="D23">
-        <v>387</v>
+        <v>12</v>
       </c>
       <c r="E23">
         <v>10398</v>
@@ -893,7 +893,7 @@
         <v>1664</v>
       </c>
       <c r="D24">
-        <v>1664</v>
+        <v>144</v>
       </c>
       <c r="E24">
         <v>50866</v>
@@ -915,7 +915,7 @@
         <v>669</v>
       </c>
       <c r="D25">
-        <v>669</v>
+        <v>24</v>
       </c>
       <c r="E25">
         <v>19350</v>
@@ -937,7 +937,7 @@
         <v>273</v>
       </c>
       <c r="D26">
-        <v>273</v>
+        <v>8</v>
       </c>
       <c r="E26">
         <v>12579</v>
@@ -959,7 +959,7 @@
         <v>447</v>
       </c>
       <c r="D27">
-        <v>447</v>
+        <v>16</v>
       </c>
       <c r="E27">
         <v>10011</v>
@@ -981,7 +981,7 @@
         <v>2596</v>
       </c>
       <c r="D28">
-        <v>2596</v>
+        <v>228</v>
       </c>
       <c r="E28">
         <v>49202</v>
@@ -1003,7 +1003,7 @@
         <v>502</v>
       </c>
       <c r="D29">
-        <v>502</v>
+        <v>28</v>
       </c>
       <c r="E29">
         <v>18681</v>
@@ -1025,7 +1025,7 @@
         <v>2411</v>
       </c>
       <c r="D30">
-        <v>2411</v>
+        <v>132</v>
       </c>
       <c r="E30">
         <v>12306</v>
@@ -1047,7 +1047,7 @@
         <v>239</v>
       </c>
       <c r="D31">
-        <v>239</v>
+        <v>11</v>
       </c>
       <c r="E31">
         <v>9564</v>
@@ -1069,7 +1069,7 @@
         <v>736</v>
       </c>
       <c r="D32">
-        <v>736</v>
+        <v>73</v>
       </c>
       <c r="E32">
         <v>46606</v>
@@ -1091,7 +1091,7 @@
         <v>421</v>
       </c>
       <c r="D33">
-        <v>421</v>
+        <v>9</v>
       </c>
       <c r="E33">
         <v>18179</v>

</xml_diff>

<commit_message>
Limit regional tests since it's not being reported anymore
</commit_message>
<xml_diff>
--- a/data/03_covid_tests/regional_tests.xlsx
+++ b/data/03_covid_tests/regional_tests.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -398,7 +398,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>43936</v>
+        <v>43932</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -412,15 +412,15 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>3.1</v>
+        <v>15399</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>43936</v>
+        <v>43932</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -428,21 +428,21 @@
         </is>
       </c>
       <c r="C3">
-        <v>0.09999999999999964</v>
+        <v>140</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>2.3</v>
+        <v>12405</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>43936</v>
+        <v>43932</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -450,21 +450,21 @@
         </is>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>693</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="E4">
-        <v>6.7</v>
+        <v>62979</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>4193</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>43936</v>
+        <v>43932</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -472,21 +472,21 @@
         </is>
       </c>
       <c r="C5">
-        <v>0.09999999999999964</v>
+        <v>239</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E5">
-        <v>4.3</v>
+        <v>22788</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>954</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>43935</v>
+        <v>43931</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -494,21 +494,21 @@
         </is>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>3.1</v>
+        <v>15399</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>479</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>43935</v>
+        <v>43931</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -516,21 +516,21 @@
         </is>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>357</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>2.2</v>
+        <v>12265</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>43935</v>
+        <v>43931</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -538,21 +538,21 @@
         </is>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1003</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="E8">
-        <v>6.7</v>
+        <v>62286</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>4125</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>43935</v>
+        <v>43931</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -560,21 +560,21 @@
         </is>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>530</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E9">
-        <v>4.2</v>
+        <v>22549</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>939</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>43934</v>
+        <v>43930</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -582,21 +582,21 @@
         </is>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>3.1</v>
+        <v>15224</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>478</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>43934</v>
+        <v>43930</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -604,21 +604,21 @@
         </is>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>223</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>2.2</v>
+        <v>11908</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>43934</v>
+        <v>43930</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -626,21 +626,21 @@
         </is>
       </c>
       <c r="C12">
-        <v>0.1000000000000005</v>
+        <v>1815</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="E12">
-        <v>6.7</v>
+        <v>61283</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>4053</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>43934</v>
+        <v>43930</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -648,21 +648,21 @@
         </is>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>479</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E13">
-        <v>4.2</v>
+        <v>22019</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>918</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>43933</v>
+        <v>43929</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -670,21 +670,21 @@
         </is>
       </c>
       <c r="C14">
-        <v>-15395.9</v>
+        <v>1792</v>
       </c>
       <c r="D14">
-        <v>-479</v>
+        <v>57</v>
       </c>
       <c r="E14">
-        <v>3.1</v>
+        <v>15071</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>478</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>43933</v>
+        <v>43929</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -692,21 +692,21 @@
         </is>
       </c>
       <c r="C15">
-        <v>-12402.8</v>
+        <v>337</v>
       </c>
       <c r="D15">
-        <v>-266</v>
+        <v>6</v>
       </c>
       <c r="E15">
-        <v>2.2</v>
+        <v>11685</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>43933</v>
+        <v>43929</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -714,21 +714,21 @@
         </is>
       </c>
       <c r="C16">
-        <v>-62972.4</v>
+        <v>1557</v>
       </c>
       <c r="D16">
-        <v>-4193</v>
+        <v>98</v>
       </c>
       <c r="E16">
-        <v>6.6</v>
+        <v>59468</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>3919</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>43933</v>
+        <v>43929</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -736,21 +736,21 @@
         </is>
       </c>
       <c r="C17">
-        <v>-22783.8</v>
+        <v>330</v>
       </c>
       <c r="D17">
-        <v>-954</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>4.2</v>
+        <v>21540</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>887</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>43932</v>
+        <v>43928</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -758,21 +758,21 @@
         </is>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>15399</v>
+        <v>13279</v>
       </c>
       <c r="F18">
-        <v>479</v>
+        <v>421</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>43932</v>
+        <v>43928</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -780,21 +780,21 @@
         </is>
       </c>
       <c r="C19">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>12405</v>
+        <v>11348</v>
       </c>
       <c r="F19">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>43932</v>
+        <v>43928</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -802,21 +802,21 @@
         </is>
       </c>
       <c r="C20">
-        <v>693</v>
+        <v>2089</v>
       </c>
       <c r="D20">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="E20">
-        <v>62979</v>
+        <v>57911</v>
       </c>
       <c r="F20">
-        <v>4193</v>
+        <v>3821</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
-        <v>43932</v>
+        <v>43928</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -824,21 +824,21 @@
         </is>
       </c>
       <c r="C21">
-        <v>239</v>
+        <v>457</v>
       </c>
       <c r="D21">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E21">
-        <v>22788</v>
+        <v>21210</v>
       </c>
       <c r="F21">
-        <v>954</v>
+        <v>881</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
-        <v>43931</v>
+        <v>43927</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -846,21 +846,21 @@
         </is>
       </c>
       <c r="C22">
-        <v>175</v>
+        <v>119</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22">
-        <v>15399</v>
+        <v>13268</v>
       </c>
       <c r="F22">
-        <v>479</v>
+        <v>421</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2">
-        <v>43931</v>
+        <v>43927</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -868,21 +868,21 @@
         </is>
       </c>
       <c r="C23">
-        <v>357</v>
+        <v>173</v>
       </c>
       <c r="D23">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E23">
-        <v>12265</v>
+        <v>11308</v>
       </c>
       <c r="F23">
-        <v>264</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2">
-        <v>43931</v>
+        <v>43927</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -890,21 +890,21 @@
         </is>
       </c>
       <c r="C24">
-        <v>1003</v>
+        <v>1254</v>
       </c>
       <c r="D24">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="E24">
-        <v>62286</v>
+        <v>55822</v>
       </c>
       <c r="F24">
-        <v>4125</v>
+        <v>3703</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2">
-        <v>43931</v>
+        <v>43927</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -912,21 +912,21 @@
         </is>
       </c>
       <c r="C25">
-        <v>530</v>
+        <v>297</v>
       </c>
       <c r="D25">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E25">
-        <v>22549</v>
+        <v>20753</v>
       </c>
       <c r="F25">
-        <v>939</v>
+        <v>871</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2">
-        <v>43930</v>
+        <v>43926</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -934,21 +934,21 @@
         </is>
       </c>
       <c r="C26">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>15224</v>
+        <v>13149</v>
       </c>
       <c r="F26">
-        <v>478</v>
+        <v>419</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
-        <v>43930</v>
+        <v>43926</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -956,21 +956,21 @@
         </is>
       </c>
       <c r="C27">
-        <v>223</v>
+        <v>408</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E27">
-        <v>11908</v>
+        <v>11135</v>
       </c>
       <c r="F27">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2">
-        <v>43930</v>
+        <v>43926</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -978,21 +978,21 @@
         </is>
       </c>
       <c r="C28">
-        <v>1815</v>
+        <v>1479</v>
       </c>
       <c r="D28">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="E28">
-        <v>61283</v>
+        <v>54568</v>
       </c>
       <c r="F28">
-        <v>4053</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2">
-        <v>43930</v>
+        <v>43926</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1000,21 +1000,21 @@
         </is>
       </c>
       <c r="C29">
-        <v>479</v>
+        <v>686</v>
       </c>
       <c r="D29">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E29">
-        <v>22019</v>
+        <v>20456</v>
       </c>
       <c r="F29">
-        <v>918</v>
+        <v>863</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2">
-        <v>43929</v>
+        <v>43925</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1022,21 +1022,21 @@
         </is>
       </c>
       <c r="C30">
-        <v>1792</v>
+        <v>244</v>
       </c>
       <c r="D30">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>15071</v>
+        <v>12967</v>
       </c>
       <c r="F30">
-        <v>478</v>
+        <v>418</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2">
-        <v>43929</v>
+        <v>43925</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1044,21 +1044,21 @@
         </is>
       </c>
       <c r="C31">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D31">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E31">
-        <v>11685</v>
+        <v>10727</v>
       </c>
       <c r="F31">
-        <v>251</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2">
-        <v>43929</v>
+        <v>43925</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1066,21 +1066,21 @@
         </is>
       </c>
       <c r="C32">
-        <v>1557</v>
+        <v>2223</v>
       </c>
       <c r="D32">
-        <v>98</v>
+        <v>157</v>
       </c>
       <c r="E32">
-        <v>59468</v>
+        <v>53089</v>
       </c>
       <c r="F32">
-        <v>3919</v>
+        <v>3455</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2">
-        <v>43929</v>
+        <v>43925</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1088,21 +1088,21 @@
         </is>
       </c>
       <c r="C33">
-        <v>330</v>
+        <v>420</v>
       </c>
       <c r="D33">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E33">
-        <v>21540</v>
+        <v>19770</v>
       </c>
       <c r="F33">
-        <v>887</v>
+        <v>829</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
-        <v>43928</v>
+        <v>43924</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1110,21 +1110,21 @@
         </is>
       </c>
       <c r="C34">
-        <v>11</v>
+        <v>144</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E34">
-        <v>13279</v>
+        <v>12723</v>
       </c>
       <c r="F34">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2">
-        <v>43928</v>
+        <v>43924</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1132,21 +1132,21 @@
         </is>
       </c>
       <c r="C35">
-        <v>40</v>
+        <v>387</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E35">
-        <v>11348</v>
+        <v>10398</v>
       </c>
       <c r="F35">
-        <v>245</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2">
-        <v>43928</v>
+        <v>43924</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1154,21 +1154,21 @@
         </is>
       </c>
       <c r="C36">
-        <v>2089</v>
+        <v>1664</v>
       </c>
       <c r="D36">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="E36">
-        <v>57911</v>
+        <v>50866</v>
       </c>
       <c r="F36">
-        <v>3821</v>
+        <v>3298</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2">
-        <v>43928</v>
+        <v>43924</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1176,21 +1176,21 @@
         </is>
       </c>
       <c r="C37">
-        <v>457</v>
+        <v>669</v>
       </c>
       <c r="D37">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E37">
-        <v>21210</v>
+        <v>19350</v>
       </c>
       <c r="F37">
-        <v>881</v>
+        <v>815</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
-        <v>43927</v>
+        <v>43923</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1198,21 +1198,21 @@
         </is>
       </c>
       <c r="C38">
-        <v>119</v>
+        <v>273</v>
       </c>
       <c r="D38">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E38">
-        <v>13268</v>
+        <v>12579</v>
       </c>
       <c r="F38">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2">
-        <v>43927</v>
+        <v>43923</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1220,21 +1220,21 @@
         </is>
       </c>
       <c r="C39">
-        <v>173</v>
+        <v>447</v>
       </c>
       <c r="D39">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E39">
-        <v>11308</v>
+        <v>10011</v>
       </c>
       <c r="F39">
-        <v>245</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2">
-        <v>43927</v>
+        <v>43923</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1242,21 +1242,21 @@
         </is>
       </c>
       <c r="C40">
-        <v>1254</v>
+        <v>2596</v>
       </c>
       <c r="D40">
-        <v>101</v>
+        <v>228</v>
       </c>
       <c r="E40">
-        <v>55822</v>
+        <v>49202</v>
       </c>
       <c r="F40">
-        <v>3703</v>
+        <v>3154</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2">
-        <v>43927</v>
+        <v>43923</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1264,21 +1264,21 @@
         </is>
       </c>
       <c r="C41">
-        <v>297</v>
+        <v>502</v>
       </c>
       <c r="D41">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E41">
-        <v>20753</v>
+        <v>18681</v>
       </c>
       <c r="F41">
-        <v>871</v>
+        <v>791</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2">
-        <v>43926</v>
+        <v>43922</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1286,21 +1286,21 @@
         </is>
       </c>
       <c r="C42">
-        <v>182</v>
+        <v>2411</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="E42">
-        <v>13149</v>
+        <v>12306</v>
       </c>
       <c r="F42">
-        <v>419</v>
+        <v>407</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2">
-        <v>43926</v>
+        <v>43922</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1308,21 +1308,21 @@
         </is>
       </c>
       <c r="C43">
-        <v>408</v>
+        <v>239</v>
       </c>
       <c r="D43">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E43">
-        <v>11135</v>
+        <v>9564</v>
       </c>
       <c r="F43">
-        <v>241</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2">
-        <v>43926</v>
+        <v>43922</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1330,21 +1330,21 @@
         </is>
       </c>
       <c r="C44">
-        <v>1479</v>
+        <v>736</v>
       </c>
       <c r="D44">
-        <v>147</v>
+        <v>73</v>
       </c>
       <c r="E44">
-        <v>54568</v>
+        <v>46606</v>
       </c>
       <c r="F44">
-        <v>3602</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2">
-        <v>43926</v>
+        <v>43922</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1352,495 +1352,143 @@
         </is>
       </c>
       <c r="C45">
-        <v>686</v>
+        <v>421</v>
       </c>
       <c r="D45">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E45">
-        <v>20456</v>
+        <v>18179</v>
       </c>
       <c r="F45">
-        <v>863</v>
+        <v>763</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2">
-        <v>43925</v>
+        <v>43921</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
           <t>Region Midt</t>
         </is>
       </c>
-      <c r="C46">
-        <v>244</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
       <c r="E46">
-        <v>12967</v>
+        <v>9895</v>
       </c>
       <c r="F46">
-        <v>418</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2">
-        <v>43925</v>
+        <v>43921</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
           <t>Region Nord</t>
         </is>
       </c>
-      <c r="C47">
-        <v>329</v>
-      </c>
-      <c r="D47">
-        <v>10</v>
-      </c>
       <c r="E47">
-        <v>10727</v>
+        <v>9325</v>
       </c>
       <c r="F47">
-        <v>237</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2">
-        <v>43925</v>
+        <v>43921</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
           <t>Region Sør-Øst</t>
         </is>
       </c>
-      <c r="C48">
-        <v>2223</v>
-      </c>
-      <c r="D48">
-        <v>157</v>
-      </c>
       <c r="E48">
-        <v>53089</v>
+        <v>45870</v>
       </c>
       <c r="F48">
-        <v>3455</v>
+        <v>2853</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2">
-        <v>43925</v>
+        <v>43921</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
           <t>Region Vest</t>
         </is>
       </c>
-      <c r="C49">
-        <v>420</v>
-      </c>
-      <c r="D49">
-        <v>14</v>
-      </c>
       <c r="E49">
-        <v>19770</v>
+        <v>17758</v>
       </c>
       <c r="F49">
-        <v>829</v>
+        <v>754</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2">
-        <v>43924</v>
+        <v>43914</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
           <t>Region Midt</t>
         </is>
       </c>
-      <c r="C50">
-        <v>144</v>
-      </c>
-      <c r="D50">
-        <v>2</v>
-      </c>
       <c r="E50">
-        <v>12723</v>
+        <v>4680</v>
       </c>
       <c r="F50">
-        <v>417</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2">
-        <v>43924</v>
+        <v>43914</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
           <t>Region Nord</t>
         </is>
       </c>
-      <c r="C51">
-        <v>387</v>
-      </c>
-      <c r="D51">
-        <v>12</v>
-      </c>
       <c r="E51">
-        <v>10398</v>
+        <v>6575</v>
       </c>
       <c r="F51">
-        <v>227</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2">
-        <v>43924</v>
+        <v>43914</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
           <t>Region Sør-Øst</t>
         </is>
       </c>
-      <c r="C52">
-        <v>1664</v>
-      </c>
-      <c r="D52">
-        <v>144</v>
-      </c>
       <c r="E52">
-        <v>50866</v>
+        <v>31303</v>
       </c>
       <c r="F52">
-        <v>3298</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2">
-        <v>43924</v>
+        <v>43914</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
           <t>Region Vest</t>
         </is>
       </c>
-      <c r="C53">
-        <v>669</v>
-      </c>
-      <c r="D53">
-        <v>24</v>
-      </c>
       <c r="E53">
-        <v>19350</v>
+        <v>13765</v>
       </c>
       <c r="F53">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="2">
-        <v>43923</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Region Midt</t>
-        </is>
-      </c>
-      <c r="C54">
-        <v>273</v>
-      </c>
-      <c r="D54">
-        <v>8</v>
-      </c>
-      <c r="E54">
-        <v>12579</v>
-      </c>
-      <c r="F54">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="2">
-        <v>43923</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Region Nord</t>
-        </is>
-      </c>
-      <c r="C55">
-        <v>447</v>
-      </c>
-      <c r="D55">
-        <v>16</v>
-      </c>
-      <c r="E55">
-        <v>10011</v>
-      </c>
-      <c r="F55">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="2">
-        <v>43923</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Region Sør-Øst</t>
-        </is>
-      </c>
-      <c r="C56">
-        <v>2596</v>
-      </c>
-      <c r="D56">
-        <v>228</v>
-      </c>
-      <c r="E56">
-        <v>49202</v>
-      </c>
-      <c r="F56">
-        <v>3154</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="2">
-        <v>43923</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Region Vest</t>
-        </is>
-      </c>
-      <c r="C57">
-        <v>502</v>
-      </c>
-      <c r="D57">
-        <v>28</v>
-      </c>
-      <c r="E57">
-        <v>18681</v>
-      </c>
-      <c r="F57">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="2">
-        <v>43922</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Region Midt</t>
-        </is>
-      </c>
-      <c r="C58">
-        <v>2411</v>
-      </c>
-      <c r="D58">
-        <v>132</v>
-      </c>
-      <c r="E58">
-        <v>12306</v>
-      </c>
-      <c r="F58">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="2">
-        <v>43922</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Region Nord</t>
-        </is>
-      </c>
-      <c r="C59">
-        <v>239</v>
-      </c>
-      <c r="D59">
-        <v>11</v>
-      </c>
-      <c r="E59">
-        <v>9564</v>
-      </c>
-      <c r="F59">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="2">
-        <v>43922</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Region Sør-Øst</t>
-        </is>
-      </c>
-      <c r="C60">
-        <v>736</v>
-      </c>
-      <c r="D60">
-        <v>73</v>
-      </c>
-      <c r="E60">
-        <v>46606</v>
-      </c>
-      <c r="F60">
-        <v>2926</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="2">
-        <v>43922</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Region Vest</t>
-        </is>
-      </c>
-      <c r="C61">
-        <v>421</v>
-      </c>
-      <c r="D61">
-        <v>9</v>
-      </c>
-      <c r="E61">
-        <v>18179</v>
-      </c>
-      <c r="F61">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="2">
-        <v>43921</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Region Midt</t>
-        </is>
-      </c>
-      <c r="E62">
-        <v>9895</v>
-      </c>
-      <c r="F62">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="2">
-        <v>43921</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Region Nord</t>
-        </is>
-      </c>
-      <c r="E63">
-        <v>9325</v>
-      </c>
-      <c r="F63">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="2">
-        <v>43921</v>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Region Sør-Øst</t>
-        </is>
-      </c>
-      <c r="E64">
-        <v>45870</v>
-      </c>
-      <c r="F64">
-        <v>2853</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="2">
-        <v>43921</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Region Vest</t>
-        </is>
-      </c>
-      <c r="E65">
-        <v>17758</v>
-      </c>
-      <c r="F65">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="2">
-        <v>43914</v>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Region Midt</t>
-        </is>
-      </c>
-      <c r="E66">
-        <v>4680</v>
-      </c>
-      <c r="F66">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="2">
-        <v>43914</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Region Nord</t>
-        </is>
-      </c>
-      <c r="E67">
-        <v>6575</v>
-      </c>
-      <c r="F67">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="2">
-        <v>43914</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Region Sør-Øst</t>
-        </is>
-      </c>
-      <c r="E68">
-        <v>31303</v>
-      </c>
-      <c r="F68">
-        <v>1488</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="2">
-        <v>43914</v>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Region Vest</t>
-        </is>
-      </c>
-      <c r="E69">
-        <v>13765</v>
-      </c>
-      <c r="F69">
         <v>520</v>
       </c>
     </row>

</xml_diff>